<commit_message>
adding in chilling hours from fig 1
</commit_message>
<xml_diff>
--- a/data/update2019/ospree_2019update_DSS.xlsx
+++ b/data/update2019/ospree_2019update_DSS.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28209"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darwinsodhi/Documents/GitHub/ospree/data/update2019/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CatherineChamberlain/Documents/git/ospree/data/update2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB375AC-A3C7-E448-86AC-55F840597126}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14740" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -19,12 +18,15 @@
     <sheet name="data_detailed" sheetId="1" r:id="rId4"/>
     <sheet name="scratch" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,20 +37,17 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Dan Flynn</author>
   </authors>
   <commentList>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5960" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5974" uniqueCount="356">
   <si>
     <t>datasetID</t>
   </si>
@@ -1156,11 +1155,14 @@
   <si>
     <t>thermaltimetohours</t>
   </si>
+  <si>
+    <t>Screen Shot 2020-04-14 at 11.51.40 AM.png</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
@@ -1317,6 +1319,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1326,8 +1330,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1689,7 +1691,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P125"/>
   <sheetViews>
     <sheetView topLeftCell="A64" workbookViewId="0">
@@ -1703,12 +1705,12 @@
     <col min="3" max="3" width="58" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>274</v>
       </c>
@@ -1719,7 +1721,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1727,7 +1729,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>126</v>
       </c>
@@ -1745,7 +1747,7 @@
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
     </row>
-    <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>127</v>
       </c>
@@ -1753,7 +1755,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>128</v>
       </c>
@@ -1761,7 +1763,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>129</v>
       </c>
@@ -1769,7 +1771,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>130</v>
       </c>
@@ -1777,7 +1779,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>131</v>
       </c>
@@ -1785,7 +1787,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>132</v>
       </c>
@@ -1793,7 +1795,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>134</v>
       </c>
@@ -1801,7 +1803,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>135</v>
       </c>
@@ -1809,7 +1811,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>136</v>
       </c>
@@ -1817,7 +1819,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>137</v>
       </c>
@@ -1825,7 +1827,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>138</v>
       </c>
@@ -1833,7 +1835,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>139</v>
       </c>
@@ -1871,7 +1873,7 @@
       </c>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>140</v>
       </c>
@@ -1879,7 +1881,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>141</v>
       </c>
@@ -1887,7 +1889,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>142</v>
       </c>
@@ -1895,12 +1897,12 @@
         <v>181</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>275</v>
       </c>
@@ -1912,7 +1914,7 @@
       <c r="A30" s="4"/>
       <c r="B30" s="6"/>
     </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>0</v>
       </c>
@@ -1920,7 +1922,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>144</v>
       </c>
@@ -1928,7 +1930,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>145</v>
       </c>
@@ -1936,7 +1938,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>146</v>
       </c>
@@ -1944,7 +1946,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>103</v>
       </c>
@@ -1952,7 +1954,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>147</v>
       </c>
@@ -1960,7 +1962,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>148</v>
       </c>
@@ -1968,7 +1970,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>149</v>
       </c>
@@ -1976,7 +1978,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>150</v>
       </c>
@@ -1984,7 +1986,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>151</v>
       </c>
@@ -1992,7 +1994,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>152</v>
       </c>
@@ -2000,7 +2002,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>153</v>
       </c>
@@ -2008,7 +2010,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>154</v>
       </c>
@@ -2016,7 +2018,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>155</v>
       </c>
@@ -2024,7 +2026,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>156</v>
       </c>
@@ -2032,7 +2034,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>157</v>
       </c>
@@ -2040,7 +2042,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>158</v>
       </c>
@@ -2048,7 +2050,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>159</v>
       </c>
@@ -2056,7 +2058,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>7</v>
       </c>
@@ -2064,7 +2066,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>136</v>
       </c>
@@ -2072,7 +2074,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>276</v>
       </c>
@@ -2080,7 +2082,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>0</v>
       </c>
@@ -2088,7 +2090,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>1</v>
       </c>
@@ -2096,7 +2098,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>54</v>
       </c>
@@ -2104,7 +2106,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>3</v>
       </c>
@@ -2112,7 +2114,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>4</v>
       </c>
@@ -2120,7 +2122,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>5</v>
       </c>
@@ -2128,7 +2130,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>7</v>
       </c>
@@ -2136,7 +2138,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>59</v>
       </c>
@@ -2144,7 +2146,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>61</v>
       </c>
@@ -2158,7 +2160,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>64</v>
       </c>
@@ -2166,7 +2168,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>67</v>
       </c>
@@ -2174,7 +2176,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>12</v>
       </c>
@@ -2182,7 +2184,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>13</v>
       </c>
@@ -2190,7 +2192,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>14</v>
       </c>
@@ -2198,7 +2200,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>15</v>
       </c>
@@ -2206,7 +2208,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>72</v>
       </c>
@@ -2214,7 +2216,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>17</v>
       </c>
@@ -2222,7 +2224,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>18</v>
       </c>
@@ -2230,7 +2232,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>19</v>
       </c>
@@ -2238,7 +2240,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>20</v>
       </c>
@@ -2246,7 +2248,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>21</v>
       </c>
@@ -2254,7 +2256,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>22</v>
       </c>
@@ -2262,7 +2264,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>23</v>
       </c>
@@ -2270,7 +2272,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>24</v>
       </c>
@@ -2278,27 +2280,27 @@
         <v>81</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B79" t="s">
         <v>82</v>
       </c>
-      <c r="C79" s="19" t="s">
+      <c r="C79" s="21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B80" t="s">
         <v>85</v>
       </c>
-      <c r="C80" s="19"/>
-    </row>
-    <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C80" s="21"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>27</v>
       </c>
@@ -2306,7 +2308,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>87</v>
       </c>
@@ -2314,7 +2316,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>29</v>
       </c>
@@ -2322,7 +2324,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>90</v>
       </c>
@@ -2330,37 +2332,37 @@
         <v>91</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B85" t="s">
         <v>93</v>
       </c>
-      <c r="C85" s="19" t="s">
+      <c r="C85" s="21" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B86" t="s">
         <v>96</v>
       </c>
-      <c r="C86" s="19"/>
-    </row>
-    <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C86" s="21"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>99</v>
       </c>
@@ -2368,7 +2370,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>101</v>
       </c>
@@ -2376,7 +2378,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>103</v>
       </c>
@@ -2384,7 +2386,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>36</v>
       </c>
@@ -2392,7 +2394,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>106</v>
       </c>
@@ -2400,7 +2402,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>38</v>
       </c>
@@ -2408,97 +2410,97 @@
         <v>108</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B96" t="s">
         <v>110</v>
       </c>
-      <c r="C96" s="19" t="s">
+      <c r="C96" s="21" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B97" t="s">
         <v>112</v>
       </c>
-      <c r="C97" s="21"/>
-    </row>
-    <row r="98" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="C97" s="23"/>
+    </row>
+    <row r="98" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B98" t="s">
         <v>113</v>
       </c>
-      <c r="C98" s="21"/>
-    </row>
-    <row r="99" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="C98" s="23"/>
+    </row>
+    <row r="99" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B99" t="s">
         <v>114</v>
       </c>
-      <c r="C99" s="21"/>
-    </row>
-    <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C99" s="23"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>115</v>
       </c>
       <c r="B100" t="s">
         <v>116</v>
       </c>
-      <c r="C100" s="19" t="s">
+      <c r="C100" s="21" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>118</v>
       </c>
       <c r="B101" t="s">
         <v>119</v>
       </c>
-      <c r="C101" s="19"/>
-    </row>
-    <row r="102" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="C101" s="21"/>
+    </row>
+    <row r="102" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>120</v>
       </c>
       <c r="B102" t="s">
         <v>121</v>
       </c>
-      <c r="C102" s="19"/>
-    </row>
-    <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C102" s="21"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B103" t="s">
         <v>123</v>
       </c>
-      <c r="C103" s="19"/>
-    </row>
-    <row r="104" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="C103" s="21"/>
+    </row>
+    <row r="104" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B104" t="s">
         <v>125</v>
       </c>
-      <c r="C104" s="19"/>
-    </row>
-    <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C104" s="21"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>294</v>
       </c>
@@ -2568,8 +2570,8 @@
       <c r="B116" s="11"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="20"/>
-      <c r="B117" s="20"/>
+      <c r="A117" s="22"/>
+      <c r="B117" s="22"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="12"/>
@@ -2622,20 +2624,15 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D63" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D63" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3097,16 +3094,11 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3257,16 +3249,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BW406"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" zoomScalePageLayoutView="90" workbookViewId="0">
@@ -37927,20 +37914,15 @@
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7:P21"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37963,7 +37945,7 @@
         <f>AVERAGE(I7,I8)</f>
         <v>81.754999999999995</v>
       </c>
-      <c r="K7" s="22">
+      <c r="K7" s="19">
         <v>41621</v>
       </c>
       <c r="M7">
@@ -37976,11 +37958,29 @@
         <f>AVERAGE(M7,N7)</f>
         <v>130.16300000000001</v>
       </c>
-      <c r="P7" s="22">
+      <c r="P7" s="19">
         <v>41621</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>355</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>9.8710000000000004</v>
+      </c>
+      <c r="E8">
+        <v>10.058</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
       <c r="I8">
         <v>81.754999999999995</v>
       </c>
@@ -37994,19 +37994,37 @@
         <f t="shared" ref="O8:O21" si="0">AVERAGE(M8,N8)</f>
         <v>140.24650000000003</v>
       </c>
-      <c r="P8" s="22">
+      <c r="P8" s="19">
         <v>41631</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>355</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>10.281000000000001</v>
+      </c>
+      <c r="E9">
+        <v>118.182</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
       <c r="I9">
         <v>93.013000000000005</v>
       </c>
       <c r="J9">
-        <f t="shared" ref="J8:J36" si="1">AVERAGE(I9,I10)</f>
+        <f t="shared" ref="J9:J35" si="1">AVERAGE(I9,I10)</f>
         <v>93.013000000000005</v>
       </c>
-      <c r="K9" s="22">
+      <c r="K9" s="19">
         <v>41631</v>
       </c>
       <c r="M9">
@@ -38019,11 +38037,29 @@
         <f t="shared" si="0"/>
         <v>150.4555</v>
       </c>
-      <c r="P9" s="22">
+      <c r="P9" s="19">
         <v>41641</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>355</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>10.742000000000001</v>
+      </c>
+      <c r="E10">
+        <v>274.08100000000002</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
       <c r="I10">
         <v>93.013000000000005</v>
       </c>
@@ -38037,11 +38073,29 @@
         <f t="shared" si="0"/>
         <v>158.42349999999999</v>
       </c>
-      <c r="P10" s="22">
+      <c r="P10" s="19">
         <v>41649</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>355</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>11.183</v>
+      </c>
+      <c r="E11">
+        <v>402.32100000000003</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
       <c r="I11">
         <v>104.27</v>
       </c>
@@ -38049,7 +38103,7 @@
         <f t="shared" si="1"/>
         <v>103.99549999999999</v>
       </c>
-      <c r="K11" s="22">
+      <c r="K11" s="19">
         <v>41641</v>
       </c>
       <c r="M11">
@@ -38062,11 +38116,29 @@
         <f t="shared" si="0"/>
         <v>168.63249999999999</v>
       </c>
-      <c r="P11" s="22">
+      <c r="P11" s="19">
         <v>41659</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>355</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>11.613</v>
+      </c>
+      <c r="E12">
+        <v>482.78500000000003</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
       <c r="I12">
         <v>103.721</v>
       </c>
@@ -38080,11 +38152,29 @@
         <f t="shared" si="0"/>
         <v>178.96600000000001</v>
       </c>
-      <c r="P12" s="22">
+      <c r="P12" s="19">
         <v>41669</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>355</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>12.054</v>
+      </c>
+      <c r="E13">
+        <v>588.39499999999998</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
       <c r="I13">
         <v>113.331</v>
       </c>
@@ -38092,7 +38182,7 @@
         <f t="shared" si="1"/>
         <v>113.0565</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="19">
         <v>41651</v>
       </c>
       <c r="M13">
@@ -38105,11 +38195,29 @@
         <f t="shared" si="0"/>
         <v>189.0505</v>
       </c>
-      <c r="P13" s="22">
+      <c r="P13" s="19">
         <v>41679</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>355</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>12.515000000000001</v>
+      </c>
+      <c r="E14">
+        <v>706.57600000000002</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
       <c r="I14">
         <v>112.782</v>
       </c>
@@ -38123,11 +38231,29 @@
         <f t="shared" si="0"/>
         <v>199.38399999999999</v>
       </c>
-      <c r="P14" s="23">
+      <c r="P14" s="20">
         <v>41689</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>355</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>12.946</v>
+      </c>
+      <c r="E15">
+        <v>716.63400000000001</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
       <c r="I15">
         <v>124.31399999999999</v>
       </c>
@@ -38135,7 +38261,7 @@
         <f t="shared" si="1"/>
         <v>124.17699999999999</v>
       </c>
-      <c r="K15" s="22">
+      <c r="K15" s="19">
         <v>41661</v>
       </c>
       <c r="M15">
@@ -38148,11 +38274,29 @@
         <f t="shared" si="0"/>
         <v>209.59200000000001</v>
       </c>
-      <c r="P15" s="23">
+      <c r="P15" s="20">
         <v>41699</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>355</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>13.407</v>
+      </c>
+      <c r="E16">
+        <v>734.23599999999999</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
       <c r="I16">
         <v>124.04</v>
       </c>
@@ -38166,11 +38310,29 @@
         <f t="shared" si="0"/>
         <v>217.809</v>
       </c>
-      <c r="P16" s="23">
+      <c r="P16" s="20">
         <v>41707</v>
       </c>
     </row>
-    <row r="17" spans="9:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>355</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>14.217000000000001</v>
+      </c>
+      <c r="E17">
+        <v>744.29399999999998</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
       <c r="I17">
         <v>135.297</v>
       </c>
@@ -38178,7 +38340,7 @@
         <f t="shared" si="1"/>
         <v>135.43450000000001</v>
       </c>
-      <c r="K17" s="22">
+      <c r="K17" s="19">
         <v>41671</v>
       </c>
       <c r="M17">
@@ -38191,11 +38353,29 @@
         <f t="shared" si="0"/>
         <v>225.9015</v>
       </c>
-      <c r="P17" s="22">
+      <c r="P17" s="19">
         <v>41716</v>
       </c>
     </row>
-    <row r="18" spans="9:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>355</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>14.647</v>
+      </c>
+      <c r="E18">
+        <v>824.75800000000004</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
       <c r="I18">
         <v>135.572</v>
       </c>
@@ -38209,11 +38389,29 @@
         <f t="shared" si="0"/>
         <v>232.12650000000002</v>
       </c>
-      <c r="P18" s="23">
+      <c r="P18" s="20">
         <v>41722</v>
       </c>
     </row>
-    <row r="19" spans="9:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>355</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>15.119</v>
+      </c>
+      <c r="E19">
+        <v>925.33799999999997</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
       <c r="I19">
         <v>146.83000000000001</v>
       </c>
@@ -38221,7 +38419,7 @@
         <f t="shared" si="1"/>
         <v>146.6925</v>
       </c>
-      <c r="K19" s="22">
+      <c r="K19" s="19">
         <v>41681</v>
       </c>
       <c r="M19">
@@ -38234,11 +38432,29 @@
         <f t="shared" si="0"/>
         <v>239.34750000000003</v>
       </c>
-      <c r="P19" s="22">
+      <c r="P19" s="19">
         <v>41729</v>
       </c>
     </row>
-    <row r="20" spans="9:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>355</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>15.548999999999999</v>
+      </c>
+      <c r="E20">
+        <v>1086.2670000000001</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
       <c r="I20">
         <v>146.55500000000001</v>
       </c>
@@ -38252,11 +38468,29 @@
         <f t="shared" si="0"/>
         <v>246.19499999999999</v>
       </c>
-      <c r="P20" s="23">
+      <c r="P20" s="20">
         <v>41736</v>
       </c>
     </row>
-    <row r="21" spans="9:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>355</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>15.98</v>
+      </c>
+      <c r="E21">
+        <v>1232.1079999999999</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
       <c r="I21">
         <v>158.08699999999999</v>
       </c>
@@ -38264,7 +38498,7 @@
         <f t="shared" si="1"/>
         <v>157.94999999999999</v>
       </c>
-      <c r="K21" s="22">
+      <c r="K21" s="19">
         <v>41691</v>
       </c>
       <c r="M21">
@@ -38277,16 +38511,16 @@
         <f t="shared" si="0"/>
         <v>254.78550000000001</v>
       </c>
-      <c r="P21" s="22">
+      <c r="P21" s="19">
         <v>41745</v>
       </c>
     </row>
-    <row r="22" spans="9:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I22">
         <v>157.81299999999999</v>
       </c>
     </row>
-    <row r="23" spans="9:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I23">
         <v>169.07</v>
       </c>
@@ -38294,17 +38528,17 @@
         <f t="shared" si="1"/>
         <v>168.93299999999999</v>
       </c>
-      <c r="K23" s="22">
+      <c r="K23" s="19">
         <v>41701</v>
       </c>
-      <c r="P23" s="22"/>
-    </row>
-    <row r="24" spans="9:16" x14ac:dyDescent="0.2">
+      <c r="P23" s="19"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I24">
         <v>168.79599999999999</v>
       </c>
     </row>
-    <row r="25" spans="9:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I25">
         <v>178.40600000000001</v>
       </c>
@@ -38312,17 +38546,17 @@
         <f t="shared" si="1"/>
         <v>178.26850000000002</v>
       </c>
-      <c r="K25" s="22">
+      <c r="K25" s="19">
         <v>41711</v>
       </c>
-      <c r="P25" s="22"/>
-    </row>
-    <row r="26" spans="9:16" x14ac:dyDescent="0.2">
+      <c r="P25" s="19"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I26">
         <v>178.131</v>
       </c>
     </row>
-    <row r="27" spans="9:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I27">
         <v>187.19200000000001</v>
       </c>
@@ -38330,17 +38564,17 @@
         <f t="shared" si="1"/>
         <v>187.19200000000001</v>
       </c>
-      <c r="K27" s="22">
+      <c r="K27" s="19">
         <v>41720</v>
       </c>
-      <c r="P27" s="22"/>
-    </row>
-    <row r="28" spans="9:16" x14ac:dyDescent="0.2">
+      <c r="P27" s="19"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I28">
         <v>187.19200000000001</v>
       </c>
     </row>
-    <row r="29" spans="9:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I29">
         <v>193.233</v>
       </c>
@@ -38348,16 +38582,16 @@
         <f t="shared" si="1"/>
         <v>193.64499999999998</v>
       </c>
-      <c r="K29" s="22">
+      <c r="K29" s="19">
         <v>41727</v>
       </c>
     </row>
-    <row r="30" spans="9:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I30">
         <v>194.05699999999999</v>
       </c>
     </row>
-    <row r="31" spans="9:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I31">
         <v>202.01900000000001</v>
       </c>
@@ -38366,7 +38600,7 @@
         <v>202.01900000000001</v>
       </c>
     </row>
-    <row r="32" spans="9:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I32">
         <v>202.01900000000001</v>
       </c>
@@ -38401,10 +38635,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>